<commit_message>
Updating BOM and router schemas.
</commit_message>
<xml_diff>
--- a/doc/midi_router-bom.xlsx
+++ b/doc/midi_router-bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max_romanov/projects/midi_router/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBBB8E4-5B19-1D47-9681-0360BF570CE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A993D024-DE54-CB4A-87A0-9CCB2D1700B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="1120" windowWidth="26340" windowHeight="15540" xr2:uid="{5426D260-D021-E24F-84F4-6AC1EB5D6F1C}"/>
+    <workbookView xWindow="1640" yWindow="1120" windowWidth="26340" windowHeight="15540" activeTab="1" xr2:uid="{5426D260-D021-E24F-84F4-6AC1EB5D6F1C}"/>
   </bookViews>
   <sheets>
     <sheet name="x4" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="253">
   <si>
     <t>id</t>
   </si>
@@ -713,6 +713,78 @@
   </si>
   <si>
     <t>15.12.2021</t>
+  </si>
+  <si>
+    <t>Стойки</t>
+  </si>
+  <si>
+    <t>Cтойки латунные 18мм</t>
+  </si>
+  <si>
+    <t>PCHSS-18</t>
+  </si>
+  <si>
+    <t>#5016317462462510</t>
+  </si>
+  <si>
+    <t>14.01.2022</t>
+  </si>
+  <si>
+    <t>Винт М3</t>
+  </si>
+  <si>
+    <t>Винт М3x6мм</t>
+  </si>
+  <si>
+    <t>M3x6</t>
+  </si>
+  <si>
+    <t>M3x6 A2 304</t>
+  </si>
+  <si>
+    <t>#5016333550992510</t>
+  </si>
+  <si>
+    <t>Саморез</t>
+  </si>
+  <si>
+    <t>Cаморез 2.6x12mm</t>
+  </si>
+  <si>
+    <t>2.6x12</t>
+  </si>
+  <si>
+    <t>2.6x12mm Pan Head</t>
+  </si>
+  <si>
+    <t>#5012498625982510</t>
+  </si>
+  <si>
+    <t>03.08.2021</t>
+  </si>
+  <si>
+    <t>HCPL2631</t>
+  </si>
+  <si>
+    <t>HCPL-2631</t>
+  </si>
+  <si>
+    <t>#5015224573612510</t>
+  </si>
+  <si>
+    <t>26.11.2021</t>
+  </si>
+  <si>
+    <t>DS1023-1x2S21</t>
+  </si>
+  <si>
+    <t>#2784510</t>
+  </si>
+  <si>
+    <t>#07769607</t>
+  </si>
+  <si>
+    <t>18.11.2022</t>
   </si>
 </sst>
 </file>
@@ -723,7 +795,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ _R_U_B"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -742,6 +814,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -855,7 +955,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -926,6 +1026,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1241,10 +1348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7993AECC-982E-A443-870E-38A46DB5AE88}">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36:K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1853,216 +1960,219 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17" s="40">
+        <v>0</v>
+      </c>
+      <c r="C17" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="41" t="s">
         <v>167</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="41" t="s">
         <v>166</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="41" t="s">
         <v>168</v>
       </c>
-      <c r="I17" s="18" t="s">
+      <c r="I17" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="40">
         <v>17.940000000000001</v>
       </c>
-      <c r="K17" s="16">
+      <c r="K17" s="43">
         <v>40</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="40">
         <v>190</v>
       </c>
-      <c r="M17" s="17">
+      <c r="M17" s="44">
         <f t="shared" si="14"/>
         <v>907.6</v>
       </c>
-      <c r="N17" s="17">
+      <c r="N17" s="44">
         <f t="shared" si="15"/>
-        <v>45.38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>59</v>
+        <v>245</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>207</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="G18" s="7"/>
       <c r="H18" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="I18" t="s">
-        <v>208</v>
+        <v>247</v>
+      </c>
+      <c r="I18" s="18" t="s">
+        <v>248</v>
       </c>
       <c r="J18">
-        <v>149.11000000000001</v>
-      </c>
-      <c r="K18">
-        <v>5</v>
+        <f>98.66/12</f>
+        <v>8.2216666666666658</v>
+      </c>
+      <c r="K18" s="16">
+        <f>12*5</f>
+        <v>60</v>
       </c>
       <c r="L18">
-        <v>317.52999999999997</v>
+        <v>196.54</v>
       </c>
       <c r="M18" s="17">
         <f t="shared" ref="M18" si="16">J18*K18+L18</f>
-        <v>1063.08</v>
-      </c>
-      <c r="N18" s="29">
+        <v>689.83999999999992</v>
+      </c>
+      <c r="N18" s="17">
         <f t="shared" ref="N18" si="17">M18/K18*B18</f>
-        <v>212.61599999999999</v>
+        <v>22.994666666666664</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F19" s="7">
-        <v>12.881309999999999</v>
+        <v>62</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>179</v>
+        <v>209</v>
       </c>
       <c r="I19" t="s">
-        <v>180</v>
+        <v>208</v>
       </c>
       <c r="J19">
-        <v>11</v>
+        <v>149.11000000000001</v>
       </c>
       <c r="K19">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="L19">
+        <v>317.52999999999997</v>
       </c>
       <c r="M19" s="17">
         <f t="shared" ref="M19" si="18">J19*K19+L19</f>
+        <v>1063.08</v>
+      </c>
+      <c r="N19" s="29">
+        <f t="shared" ref="N19" si="19">M19/K19*B19</f>
+        <v>212.61599999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="7">
+        <v>12.881309999999999</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="I20" t="s">
+        <v>180</v>
+      </c>
+      <c r="J20">
+        <v>11</v>
+      </c>
+      <c r="K20">
+        <v>10</v>
+      </c>
+      <c r="M20" s="17">
+        <f t="shared" ref="M20" si="20">J20*K20+L20</f>
         <v>110</v>
       </c>
-      <c r="N19" s="17">
-        <f t="shared" ref="N19" si="19">M19/K19*B19</f>
+      <c r="N20" s="17">
+        <f t="shared" ref="N20" si="21">M20/K20*B20</f>
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="31" t="s">
+    <row r="21" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="31"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>189</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="I21" t="s">
-        <v>180</v>
-      </c>
-      <c r="J21">
-        <v>0.4</v>
-      </c>
-      <c r="K21">
-        <v>100</v>
-      </c>
-      <c r="M21" s="17">
-        <f t="shared" ref="M21:M22" si="20">J21*K21+L21</f>
-        <v>40</v>
-      </c>
-      <c r="N21" s="17">
-        <f t="shared" ref="N21:N22" si="21">M21/K21*B21</f>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>22</v>
+        <v>190</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>24</v>
+      <c r="F22" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>179</v>
@@ -2071,40 +2181,41 @@
         <v>180</v>
       </c>
       <c r="J22">
-        <v>0.47</v>
-      </c>
-      <c r="K22" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="K22">
         <v>100</v>
       </c>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13">
-        <f t="shared" si="20"/>
-        <v>47</v>
-      </c>
-      <c r="N22" s="14">
-        <f t="shared" si="21"/>
-        <v>0.47</v>
+      <c r="M22" s="17">
+        <f t="shared" ref="M22:M23" si="22">J22*K22+L22</f>
+        <v>40</v>
+      </c>
+      <c r="N22" s="17">
+        <f t="shared" ref="N22:N23" si="23">M22/K22*B22</f>
+        <v>0.4</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="24" t="s">
-        <v>87</v>
+      <c r="A23" s="15" t="s">
+        <v>21</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>192</v>
-      </c>
-      <c r="D23" s="23"/>
+        <v>191</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="E23" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="G23" s="26" t="s">
-        <v>193</v>
+      <c r="F23" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>179</v>
@@ -2113,42 +2224,40 @@
         <v>180</v>
       </c>
       <c r="J23">
-        <v>0.86</v>
-      </c>
-      <c r="K23" s="16">
+        <v>0.47</v>
+      </c>
+      <c r="K23" s="8">
         <v>100</v>
       </c>
-      <c r="L23" s="27"/>
+      <c r="L23" s="13"/>
       <c r="M23" s="13">
-        <f t="shared" ref="M23:M25" si="22">J23*K23+L23</f>
-        <v>86</v>
+        <f t="shared" si="22"/>
+        <v>47</v>
       </c>
       <c r="N23" s="14">
-        <f t="shared" ref="N23:N25" si="23">M23/K23*B23</f>
-        <v>0.86</v>
+        <f t="shared" si="23"/>
+        <v>0.47</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="24" t="s">
-        <v>132</v>
+        <v>87</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>133</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>195</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="D24" s="23"/>
       <c r="E24" s="6" t="s">
-        <v>134</v>
+        <v>18</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>132</v>
+        <v>194</v>
       </c>
       <c r="G24" s="26" t="s">
-        <v>135</v>
+        <v>193</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>179</v>
@@ -2157,166 +2266,167 @@
         <v>180</v>
       </c>
       <c r="J24">
+        <v>0.86</v>
+      </c>
+      <c r="K24" s="16">
+        <v>100</v>
+      </c>
+      <c r="L24" s="27"/>
+      <c r="M24" s="13">
+        <f t="shared" ref="M24:M26" si="24">J24*K24+L24</f>
+        <v>86</v>
+      </c>
+      <c r="N24" s="14">
+        <f t="shared" ref="N24:N26" si="25">M24/K24*B24</f>
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>133</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="G25" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="I25" t="s">
+        <v>180</v>
+      </c>
+      <c r="J25">
         <v>3.2</v>
       </c>
-      <c r="K24" s="16">
+      <c r="K25" s="16">
         <v>10</v>
       </c>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27">
-        <f t="shared" si="22"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="27">
+        <f t="shared" si="24"/>
         <v>32</v>
       </c>
-      <c r="N24" s="27">
-        <f t="shared" si="23"/>
+      <c r="N25" s="27">
+        <f t="shared" si="25"/>
         <v>3.2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B26">
         <v>0.25</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>36</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>78</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F26" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G26" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="H26" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I26" t="s">
         <v>185</v>
       </c>
-      <c r="J25">
+      <c r="J26">
         <v>45</v>
       </c>
-      <c r="K25" s="16">
+      <c r="K26" s="16">
         <v>5</v>
       </c>
-      <c r="M25" s="17">
-        <f t="shared" si="22"/>
+      <c r="M26" s="17">
+        <f t="shared" si="24"/>
         <v>225</v>
       </c>
-      <c r="N25" s="17">
-        <f t="shared" si="23"/>
+      <c r="N26" s="17">
+        <f t="shared" si="25"/>
         <v>11.25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B26">
-        <v>8</v>
-      </c>
-      <c r="C26" t="s">
-        <v>196</v>
-      </c>
-      <c r="D26" t="s">
-        <v>136</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="I26" t="s">
-        <v>199</v>
-      </c>
-      <c r="J26">
-        <v>7.3760000000000003</v>
-      </c>
-      <c r="K26" s="16">
-        <v>100</v>
-      </c>
-      <c r="L26">
-        <v>775.44</v>
-      </c>
-      <c r="M26" s="17">
-        <f t="shared" ref="M26:M33" si="24">J26*K26+L26</f>
-        <v>1513.04</v>
-      </c>
-      <c r="N26" s="17">
-        <f t="shared" ref="N26:N33" si="25">M26/K26*B26</f>
-        <v>121.0432</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>109</v>
+        <v>172</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D27" t="s">
-        <v>111</v>
-      </c>
-      <c r="E27"/>
+        <v>136</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>137</v>
+      </c>
       <c r="F27" s="7" t="s">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>139</v>
+        <v>197</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>179</v>
+        <v>198</v>
       </c>
       <c r="I27" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="J27">
-        <v>6</v>
-      </c>
-      <c r="K27">
-        <v>10</v>
+        <v>7.3760000000000003</v>
+      </c>
+      <c r="K27" s="16">
+        <v>100</v>
+      </c>
+      <c r="L27">
+        <v>775.44</v>
       </c>
       <c r="M27" s="17">
-        <f t="shared" si="24"/>
-        <v>60</v>
+        <f t="shared" ref="M27:M37" si="26">J27*K27+L27</f>
+        <v>1513.04</v>
       </c>
       <c r="N27" s="17">
-        <f t="shared" si="25"/>
-        <v>6</v>
+        <f t="shared" ref="N27:N37" si="27">M27/K27*B27</f>
+        <v>121.0432</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>203</v>
+        <v>109</v>
       </c>
       <c r="B28">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D28" t="s">
-        <v>96</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>18</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="E28"/>
       <c r="F28" s="7" t="s">
-        <v>205</v>
+        <v>140</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>204</v>
+        <v>139</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>179</v>
@@ -2325,41 +2435,41 @@
         <v>180</v>
       </c>
       <c r="J28">
-        <v>0.12</v>
+        <v>6</v>
       </c>
       <c r="K28">
-        <v>120</v>
+        <v>10</v>
       </c>
       <c r="M28" s="17">
-        <f t="shared" si="24"/>
-        <v>14.399999999999999</v>
+        <f t="shared" si="26"/>
+        <v>60</v>
       </c>
       <c r="N28" s="17">
-        <f t="shared" si="25"/>
-        <v>1.4399999999999997</v>
+        <f t="shared" si="27"/>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>112</v>
+      <c r="A29" s="6" t="s">
+        <v>203</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D29" t="s">
-        <v>114</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>115</v>
+        <v>96</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>112</v>
+        <v>205</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>151</v>
+        <v>204</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>179</v>
@@ -2368,125 +2478,140 @@
         <v>180</v>
       </c>
       <c r="J29">
-        <v>6.3</v>
+        <v>0.12</v>
       </c>
       <c r="K29">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="M29" s="17">
-        <f t="shared" si="24"/>
-        <v>63</v>
+        <f t="shared" si="26"/>
+        <v>14.399999999999999</v>
       </c>
       <c r="N29" s="17">
-        <f t="shared" si="25"/>
-        <v>6.3</v>
+        <f t="shared" si="27"/>
+        <v>1.4399999999999997</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="D30" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>153</v>
+        <v>112</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="I30" s="18" t="s">
-        <v>119</v>
+        <v>179</v>
+      </c>
+      <c r="I30" t="s">
+        <v>180</v>
       </c>
       <c r="J30">
-        <v>10.8</v>
+        <v>6.3</v>
       </c>
       <c r="K30">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="M30" s="17">
-        <f t="shared" si="24"/>
-        <v>216</v>
+        <f t="shared" si="26"/>
+        <v>63</v>
       </c>
       <c r="N30" s="17">
-        <f t="shared" si="25"/>
-        <v>10.8</v>
+        <f t="shared" si="27"/>
+        <v>6.3</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
-        <v>173</v>
+      <c r="A31" t="s">
+        <v>106</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
+      <c r="C31" t="s">
+        <v>206</v>
+      </c>
+      <c r="D31" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="I31" s="18" t="s">
+        <v>119</v>
+      </c>
       <c r="J31">
+        <v>10.8</v>
+      </c>
+      <c r="K31">
+        <v>20</v>
+      </c>
+      <c r="M31" s="17">
+        <f t="shared" si="26"/>
+        <v>216</v>
+      </c>
+      <c r="N31" s="17">
+        <f t="shared" si="27"/>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="J32">
         <v>75.724000000000004</v>
       </c>
-      <c r="K31">
+      <c r="K32">
         <v>10</v>
       </c>
-      <c r="L31">
+      <c r="L32">
         <v>729.22</v>
       </c>
-      <c r="M31" s="17">
-        <f t="shared" si="24"/>
+      <c r="M32" s="17">
+        <f t="shared" si="26"/>
         <v>1486.46</v>
       </c>
-      <c r="N31" s="17">
-        <f t="shared" si="25"/>
+      <c r="N32" s="17">
+        <f t="shared" si="27"/>
         <v>148.64600000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>174</v>
       </c>
-      <c r="B32">
+      <c r="B33">
         <v>70</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>177</v>
-      </c>
-      <c r="E32"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="18"/>
-      <c r="J32">
-        <f>4400/750</f>
-        <v>5.8666666666666663</v>
-      </c>
-      <c r="K32">
-        <v>750</v>
-      </c>
-      <c r="M32" s="17">
-        <f t="shared" si="24"/>
-        <v>4400</v>
-      </c>
-      <c r="N32" s="17">
-        <f t="shared" si="25"/>
-        <v>410.66666666666663</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>215</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
       </c>
       <c r="E33"/>
       <c r="F33" s="7"/>
@@ -2494,46 +2619,188 @@
       <c r="H33" s="7"/>
       <c r="I33" s="18"/>
       <c r="J33">
+        <f>4400/750</f>
+        <v>5.8666666666666663</v>
+      </c>
+      <c r="K33">
+        <v>750</v>
+      </c>
+      <c r="M33" s="17">
+        <f t="shared" si="26"/>
+        <v>4400</v>
+      </c>
+      <c r="N33" s="17">
+        <f t="shared" si="27"/>
+        <v>410.66666666666663</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>229</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>230</v>
+      </c>
+      <c r="E34" s="38" t="s">
+        <v>231</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="I34" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="J34">
+        <v>15.9</v>
+      </c>
+      <c r="K34">
+        <v>20</v>
+      </c>
+      <c r="M34" s="17">
+        <f t="shared" ref="M34:M36" si="28">J34*K34+L34</f>
+        <v>318</v>
+      </c>
+      <c r="N34" s="17">
+        <f t="shared" ref="N34:N36" si="29">M34/K34*B34</f>
+        <v>31.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>234</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>235</v>
+      </c>
+      <c r="E35" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="I35" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="J35">
+        <v>1.6434</v>
+      </c>
+      <c r="K35">
+        <v>100</v>
+      </c>
+      <c r="M35" s="17">
+        <f t="shared" si="28"/>
+        <v>164.34</v>
+      </c>
+      <c r="N35" s="17">
+        <f t="shared" si="29"/>
+        <v>6.5735999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>239</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>240</v>
+      </c>
+      <c r="E36" s="38" t="s">
+        <v>241</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="I36" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="J36">
+        <v>1.4508000000000001</v>
+      </c>
+      <c r="K36">
+        <v>100</v>
+      </c>
+      <c r="M36" s="17">
+        <f t="shared" si="28"/>
+        <v>145.08000000000001</v>
+      </c>
+      <c r="N36" s="17">
+        <f t="shared" si="29"/>
+        <v>5.8032000000000004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>215</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="E37"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="18"/>
+      <c r="J37">
         <v>10</v>
       </c>
-      <c r="K33">
+      <c r="K37">
         <v>1</v>
       </c>
-      <c r="M33" s="17">
-        <f t="shared" si="24"/>
+      <c r="M37" s="17">
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
-      <c r="N33" s="17">
-        <f t="shared" si="25"/>
+      <c r="N37" s="17">
+        <f t="shared" si="27"/>
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34" s="19" t="s">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="20">
-        <f>SUM(N4:N33)</f>
-        <v>1149.5528666666664</v>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="20">
+        <f>SUM(N4:N37)</f>
+        <v>1171.3443333333332</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="H1:N1"/>
     <mergeCell ref="A3:N3"/>
-    <mergeCell ref="A20:N20"/>
+    <mergeCell ref="A21:N21"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -2550,13 +2817,13 @@
     <hyperlink ref="G6" r:id="rId6" xr:uid="{DB881ABC-56D6-7E4A-BEBA-1E066F2C2F07}"/>
     <hyperlink ref="G7" r:id="rId7" xr:uid="{09B0C8F9-2800-B54A-A4F4-3D562E3E6FDF}"/>
     <hyperlink ref="G9" r:id="rId8" xr:uid="{096D15C7-8BBF-BB4E-84C8-35DBD788E0E2}"/>
-    <hyperlink ref="G19" r:id="rId9" xr:uid="{DB7F1783-C48C-9D40-BBFD-8D4097BE8A98}"/>
+    <hyperlink ref="G20" r:id="rId9" xr:uid="{DB7F1783-C48C-9D40-BBFD-8D4097BE8A98}"/>
     <hyperlink ref="F11" r:id="rId10" xr:uid="{F3C03C8C-0C40-094E-9F71-1C4D58A71430}"/>
     <hyperlink ref="G11" r:id="rId11" xr:uid="{1435EFC7-D123-A349-9347-F1FC07C520F3}"/>
     <hyperlink ref="F16" r:id="rId12" xr:uid="{8859AF1F-13E4-8342-B316-410A6FA0149A}"/>
     <hyperlink ref="G16" r:id="rId13" xr:uid="{AB88F6E6-123F-9D4E-9FA0-814ED4CC1BBB}"/>
-    <hyperlink ref="F25" r:id="rId14" xr:uid="{73ECD750-DE83-3146-94A2-DE706EEE6120}"/>
-    <hyperlink ref="G25" r:id="rId15" xr:uid="{8A1760EB-8876-864C-8DE1-93EE8FD52879}"/>
+    <hyperlink ref="F26" r:id="rId14" xr:uid="{73ECD750-DE83-3146-94A2-DE706EEE6120}"/>
+    <hyperlink ref="G26" r:id="rId15" xr:uid="{8A1760EB-8876-864C-8DE1-93EE8FD52879}"/>
     <hyperlink ref="H4" r:id="rId16" xr:uid="{919B0B41-0EEF-5144-B8D8-548C261081BD}"/>
     <hyperlink ref="H5" r:id="rId17" xr:uid="{756B715C-9A28-7845-BD5E-052D2A290691}"/>
     <hyperlink ref="H6" r:id="rId18" xr:uid="{FA50EF8A-3D4D-7D40-B0FE-ECD3C6EC8DEF}"/>
@@ -2572,38 +2839,38 @@
     <hyperlink ref="F12" r:id="rId28" xr:uid="{DFD91A03-B82B-1D48-B3E9-83EAD6BF2C2C}"/>
     <hyperlink ref="H12" r:id="rId29" xr:uid="{7A4372D7-3EFB-EC4E-9EE3-3A2A8D8126B4}"/>
     <hyperlink ref="H16" r:id="rId30" xr:uid="{7362C77B-1107-1940-A06A-7024A3CCD0D0}"/>
-    <hyperlink ref="F19" r:id="rId31" display="12.88131" xr:uid="{20FF9D00-0B3A-E846-9C31-D49FD05FD6B6}"/>
-    <hyperlink ref="H19" r:id="rId32" xr:uid="{B3379768-D2F2-BF4D-A818-86EFE9315E5A}"/>
-    <hyperlink ref="G21" r:id="rId33" xr:uid="{1C5104A6-6A04-4E4C-9172-DC4A512FC675}"/>
-    <hyperlink ref="H21" r:id="rId34" xr:uid="{51D7A6CF-4351-1942-B212-00AA57470581}"/>
-    <hyperlink ref="F21" r:id="rId35" xr:uid="{26939209-0E3D-B54E-8C9D-75621A567990}"/>
-    <hyperlink ref="F22" r:id="rId36" xr:uid="{CA106586-87D6-214A-B1FC-F3C165E18487}"/>
-    <hyperlink ref="G22" r:id="rId37" xr:uid="{E6710FD0-D751-E14C-83CA-F3FD3FE4D2BC}"/>
-    <hyperlink ref="H22" r:id="rId38" xr:uid="{58E74E8C-7CCB-784D-9D3F-ABCDFE44374B}"/>
-    <hyperlink ref="G23" r:id="rId39" xr:uid="{9C7B8CA6-6F7C-E44C-8EB8-CE6D10B19524}"/>
-    <hyperlink ref="H23" r:id="rId40" xr:uid="{2E3F94E3-08E8-4642-86E8-A49AEC6EA2B2}"/>
-    <hyperlink ref="F23" r:id="rId41" xr:uid="{323EEAE0-9E09-B54B-81E7-5234305BCBBB}"/>
-    <hyperlink ref="G24" r:id="rId42" xr:uid="{A2B16C39-D2E8-8344-9089-0426E4B000E5}"/>
-    <hyperlink ref="F24" r:id="rId43" xr:uid="{9D2F8C2A-510B-F843-8858-6672BBE4E308}"/>
-    <hyperlink ref="H24" r:id="rId44" xr:uid="{DA789950-489E-0946-A600-B1AE25B7E0F7}"/>
-    <hyperlink ref="H25" r:id="rId45" xr:uid="{C3363112-9F34-0A40-98C0-10727C294532}"/>
-    <hyperlink ref="G26" r:id="rId46" xr:uid="{A2FCC638-00F8-4947-AB0E-0372A59900B5}"/>
-    <hyperlink ref="H26" r:id="rId47" xr:uid="{B6A26CD5-416E-4746-993C-A5F51FB469F8}"/>
-    <hyperlink ref="G27" r:id="rId48" xr:uid="{6DDCA5D0-75BE-3E4F-B558-39A147FC422F}"/>
-    <hyperlink ref="F27" r:id="rId49" xr:uid="{C3042CE6-7315-AA4B-995F-46EC0EBC8387}"/>
-    <hyperlink ref="G29" r:id="rId50" xr:uid="{E0F917C4-4623-214A-8535-330FA265216D}"/>
-    <hyperlink ref="F29" r:id="rId51" xr:uid="{155493C7-E8C5-9C4D-A72B-897AC9F14B1C}"/>
-    <hyperlink ref="H27" r:id="rId52" xr:uid="{B680FEF0-7D1E-D84B-9F4E-806373C4079C}"/>
-    <hyperlink ref="H29" r:id="rId53" xr:uid="{C7ACB124-85BB-D348-87FC-DF98A5496B39}"/>
-    <hyperlink ref="G28" r:id="rId54" xr:uid="{CFB8644E-D50A-2145-AC8C-49872EC8CBA6}"/>
-    <hyperlink ref="F28" r:id="rId55" xr:uid="{58FF340F-D8B5-3140-9DA4-F98E1825DC1E}"/>
-    <hyperlink ref="H28" r:id="rId56" xr:uid="{D04D4D0F-31EB-4240-B5D1-EA46F62220B9}"/>
-    <hyperlink ref="G30" r:id="rId57" xr:uid="{D7AEEF35-CE08-BB49-84A0-EDE28B1BD449}"/>
-    <hyperlink ref="F30" r:id="rId58" xr:uid="{D412AE4F-8A1A-A34A-8500-C11724A83B41}"/>
-    <hyperlink ref="H30" r:id="rId59" display="https://www.terraelectronica.ru/order/07655639" xr:uid="{6988CE38-5B4C-5A44-B34A-4CEDEC17CC62}"/>
-    <hyperlink ref="F26" r:id="rId60" display="#1005002434565701" xr:uid="{60F5B472-D8C6-0F42-A138-FBC19E447B90}"/>
-    <hyperlink ref="G18" r:id="rId61" xr:uid="{A341060E-AE92-7040-A076-F3A58957D0E9}"/>
-    <hyperlink ref="H18" r:id="rId62" xr:uid="{589AE4B7-02BB-B744-B490-4C2F7DC3EC8C}"/>
+    <hyperlink ref="F20" r:id="rId31" display="12.88131" xr:uid="{20FF9D00-0B3A-E846-9C31-D49FD05FD6B6}"/>
+    <hyperlink ref="H20" r:id="rId32" xr:uid="{B3379768-D2F2-BF4D-A818-86EFE9315E5A}"/>
+    <hyperlink ref="G22" r:id="rId33" xr:uid="{1C5104A6-6A04-4E4C-9172-DC4A512FC675}"/>
+    <hyperlink ref="H22" r:id="rId34" xr:uid="{51D7A6CF-4351-1942-B212-00AA57470581}"/>
+    <hyperlink ref="F22" r:id="rId35" xr:uid="{26939209-0E3D-B54E-8C9D-75621A567990}"/>
+    <hyperlink ref="F23" r:id="rId36" xr:uid="{CA106586-87D6-214A-B1FC-F3C165E18487}"/>
+    <hyperlink ref="G23" r:id="rId37" xr:uid="{E6710FD0-D751-E14C-83CA-F3FD3FE4D2BC}"/>
+    <hyperlink ref="H23" r:id="rId38" xr:uid="{58E74E8C-7CCB-784D-9D3F-ABCDFE44374B}"/>
+    <hyperlink ref="G24" r:id="rId39" xr:uid="{9C7B8CA6-6F7C-E44C-8EB8-CE6D10B19524}"/>
+    <hyperlink ref="H24" r:id="rId40" xr:uid="{2E3F94E3-08E8-4642-86E8-A49AEC6EA2B2}"/>
+    <hyperlink ref="F24" r:id="rId41" xr:uid="{323EEAE0-9E09-B54B-81E7-5234305BCBBB}"/>
+    <hyperlink ref="G25" r:id="rId42" xr:uid="{A2B16C39-D2E8-8344-9089-0426E4B000E5}"/>
+    <hyperlink ref="F25" r:id="rId43" xr:uid="{9D2F8C2A-510B-F843-8858-6672BBE4E308}"/>
+    <hyperlink ref="H25" r:id="rId44" xr:uid="{DA789950-489E-0946-A600-B1AE25B7E0F7}"/>
+    <hyperlink ref="H26" r:id="rId45" xr:uid="{C3363112-9F34-0A40-98C0-10727C294532}"/>
+    <hyperlink ref="G27" r:id="rId46" xr:uid="{A2FCC638-00F8-4947-AB0E-0372A59900B5}"/>
+    <hyperlink ref="H27" r:id="rId47" xr:uid="{B6A26CD5-416E-4746-993C-A5F51FB469F8}"/>
+    <hyperlink ref="G28" r:id="rId48" xr:uid="{6DDCA5D0-75BE-3E4F-B558-39A147FC422F}"/>
+    <hyperlink ref="F28" r:id="rId49" xr:uid="{C3042CE6-7315-AA4B-995F-46EC0EBC8387}"/>
+    <hyperlink ref="G30" r:id="rId50" xr:uid="{E0F917C4-4623-214A-8535-330FA265216D}"/>
+    <hyperlink ref="F30" r:id="rId51" xr:uid="{155493C7-E8C5-9C4D-A72B-897AC9F14B1C}"/>
+    <hyperlink ref="H28" r:id="rId52" xr:uid="{B680FEF0-7D1E-D84B-9F4E-806373C4079C}"/>
+    <hyperlink ref="H30" r:id="rId53" xr:uid="{C7ACB124-85BB-D348-87FC-DF98A5496B39}"/>
+    <hyperlink ref="G29" r:id="rId54" xr:uid="{CFB8644E-D50A-2145-AC8C-49872EC8CBA6}"/>
+    <hyperlink ref="F29" r:id="rId55" xr:uid="{58FF340F-D8B5-3140-9DA4-F98E1825DC1E}"/>
+    <hyperlink ref="H29" r:id="rId56" xr:uid="{D04D4D0F-31EB-4240-B5D1-EA46F62220B9}"/>
+    <hyperlink ref="G31" r:id="rId57" xr:uid="{D7AEEF35-CE08-BB49-84A0-EDE28B1BD449}"/>
+    <hyperlink ref="F31" r:id="rId58" xr:uid="{D412AE4F-8A1A-A34A-8500-C11724A83B41}"/>
+    <hyperlink ref="H31" r:id="rId59" display="https://www.terraelectronica.ru/order/07655639" xr:uid="{6988CE38-5B4C-5A44-B34A-4CEDEC17CC62}"/>
+    <hyperlink ref="F27" r:id="rId60" display="#1005002434565701" xr:uid="{60F5B472-D8C6-0F42-A138-FBC19E447B90}"/>
+    <hyperlink ref="G19" r:id="rId61" xr:uid="{A341060E-AE92-7040-A076-F3A58957D0E9}"/>
+    <hyperlink ref="H19" r:id="rId62" xr:uid="{589AE4B7-02BB-B744-B490-4C2F7DC3EC8C}"/>
     <hyperlink ref="G17" r:id="rId63" xr:uid="{B1E3B80F-1202-BA4C-BA66-DD6911A4E681}"/>
     <hyperlink ref="F17" r:id="rId64" xr:uid="{4BA56443-565C-3846-9F35-F5DB491ACDFF}"/>
     <hyperlink ref="H17" r:id="rId65" xr:uid="{5FCA809F-25E0-5E4A-9F36-0754C078D8C6}"/>
@@ -2615,6 +2882,14 @@
     <hyperlink ref="H14" r:id="rId71" display="https://www.terraelectronica.ru/order/07655639" xr:uid="{07D4CAB9-6DE4-1D4C-BE7A-495B303E8093}"/>
     <hyperlink ref="G10" r:id="rId72" xr:uid="{5CDDDAD7-B779-1A4A-8B46-DFA995A894C7}"/>
     <hyperlink ref="H10" r:id="rId73" xr:uid="{C62F9978-532C-8B4C-9A76-4CA32AAF5503}"/>
+    <hyperlink ref="F34" r:id="rId74" xr:uid="{39C4633A-F7C4-6842-8464-D4C2F245FED7}"/>
+    <hyperlink ref="H34" r:id="rId75" xr:uid="{7763E51A-D819-F045-9402-F06FCBC75038}"/>
+    <hyperlink ref="F35" r:id="rId76" xr:uid="{8D250964-B9E5-6A4A-8A18-0350B7626A19}"/>
+    <hyperlink ref="H35" r:id="rId77" xr:uid="{5C282405-4A13-674D-B571-CE6CBA03851F}"/>
+    <hyperlink ref="F36" r:id="rId78" xr:uid="{3668F34B-290B-DC4D-A729-8888A59E0775}"/>
+    <hyperlink ref="H36" r:id="rId79" xr:uid="{A89DBE48-6666-F24E-A1CC-3F2566097C83}"/>
+    <hyperlink ref="F18" r:id="rId80" xr:uid="{D03F2A35-390C-EE48-9FFE-9AAC15E9E1D6}"/>
+    <hyperlink ref="H18" r:id="rId81" xr:uid="{DD8C00E6-DC97-CF43-9915-4AFF85DAFBA4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2622,10 +2897,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C343BB3-294E-094C-B28F-3093B9AA3184}">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3423,156 +3698,159 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="B20">
-        <v>4</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B20" s="40">
+        <v>0</v>
+      </c>
+      <c r="C20" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="41" t="s">
         <v>167</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="41" t="s">
         <v>166</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="H20" s="41" t="s">
         <v>168</v>
       </c>
-      <c r="I20" s="18" t="s">
+      <c r="I20" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="40">
         <v>17.940000000000001</v>
       </c>
-      <c r="K20" s="16">
+      <c r="K20" s="43">
         <v>40</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="40">
         <v>190</v>
       </c>
-      <c r="M20" s="17">
+      <c r="M20" s="44">
         <f t="shared" ref="M20" si="10">J20*K20+L20</f>
         <v>907.6</v>
       </c>
-      <c r="N20" s="17">
+      <c r="N20" s="44">
         <f t="shared" ref="N20" si="11">M20/K20*B20</f>
-        <v>90.76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>103</v>
+        <v>245</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>105</v>
+        <v>58</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>160</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="G21" s="7"/>
       <c r="H21" s="7" t="s">
-        <v>161</v>
+        <v>247</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>162</v>
+        <v>248</v>
       </c>
       <c r="J21">
-        <v>1650</v>
-      </c>
-      <c r="K21">
-        <v>10</v>
+        <f>98.66/12</f>
+        <v>8.2216666666666658</v>
+      </c>
+      <c r="K21" s="16">
+        <f>12*5</f>
+        <v>60</v>
+      </c>
+      <c r="L21">
+        <v>196.54</v>
       </c>
       <c r="M21" s="17">
         <f t="shared" ref="M21" si="12">J21*K21+L21</f>
-        <v>16500</v>
-      </c>
-      <c r="N21" s="29">
+        <v>689.83999999999992</v>
+      </c>
+      <c r="N21" s="17">
         <f t="shared" ref="N21" si="13">M21/K21*B21</f>
-        <v>1650</v>
+        <v>45.989333333333327</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="D22" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="7">
-        <v>12.880089999999999</v>
+        <v>62</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>118</v>
+        <v>161</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>119</v>
+        <v>162</v>
       </c>
       <c r="J22">
-        <v>18.7</v>
+        <v>1650</v>
       </c>
       <c r="K22">
         <v>10</v>
       </c>
       <c r="M22" s="17">
-        <f t="shared" ref="M22:M23" si="14">J22*K22+L22</f>
-        <v>187</v>
-      </c>
-      <c r="N22" s="17">
-        <f t="shared" ref="N22:N23" si="15">M22/K22*B22</f>
-        <v>18.7</v>
+        <f t="shared" ref="M22" si="14">J22*K22+L22</f>
+        <v>16500</v>
+      </c>
+      <c r="N22" s="29">
+        <f t="shared" ref="N22" si="15">M22/K22*B22</f>
+        <v>1650</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>106</v>
+      <c r="A23" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D23" t="s">
-        <v>107</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>153</v>
+        <v>66</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="7">
+        <v>12.880089999999999</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>118</v>
@@ -3581,38 +3859,41 @@
         <v>119</v>
       </c>
       <c r="J23">
-        <v>10.8</v>
+        <v>18.7</v>
       </c>
       <c r="K23">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="M23" s="17">
-        <f t="shared" si="14"/>
-        <v>216</v>
+        <f t="shared" ref="M23:M24" si="16">J23*K23+L23</f>
+        <v>187</v>
       </c>
       <c r="N23" s="17">
-        <f t="shared" si="15"/>
-        <v>10.8</v>
+        <f t="shared" ref="N23:N24" si="17">M23/K23*B23</f>
+        <v>18.7</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>109</v>
+      <c r="A24" t="s">
+        <v>106</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
-        <v>111</v>
+        <v>107</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>118</v>
@@ -3621,41 +3902,38 @@
         <v>119</v>
       </c>
       <c r="J24">
-        <v>5.7</v>
+        <v>10.8</v>
       </c>
       <c r="K24">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="M24" s="17">
-        <f t="shared" ref="M24:M26" si="16">J24*K24+L24</f>
-        <v>57</v>
+        <f t="shared" si="16"/>
+        <v>216</v>
       </c>
       <c r="N24" s="17">
-        <f t="shared" ref="N24:N26" si="17">M24/K24*B24</f>
-        <v>5.7</v>
+        <f t="shared" si="17"/>
+        <v>10.8</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>112</v>
+      <c r="A25" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D25" t="s">
-        <v>114</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>118</v>
@@ -3664,235 +3942,357 @@
         <v>119</v>
       </c>
       <c r="J25">
-        <v>5.3</v>
+        <v>5.7</v>
       </c>
       <c r="K25">
         <v>10</v>
       </c>
       <c r="M25" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="M25:M27" si="18">J25*K25+L25</f>
+        <v>57</v>
+      </c>
+      <c r="N25" s="17">
+        <f t="shared" ref="N25:N27" si="19">M25/K25*B25</f>
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>113</v>
+      </c>
+      <c r="D26" t="s">
+        <v>114</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="J26">
+        <v>5.3</v>
+      </c>
+      <c r="K26">
+        <v>10</v>
+      </c>
+      <c r="M26" s="17">
+        <f t="shared" si="18"/>
         <v>53</v>
       </c>
-      <c r="N25" s="17">
-        <f t="shared" si="17"/>
+      <c r="N26" s="17">
+        <f t="shared" si="19"/>
         <v>5.3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B26">
-        <v>14</v>
-      </c>
-      <c r="C26" t="s">
-        <v>157</v>
-      </c>
-      <c r="D26" t="s">
-        <v>136</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="I26" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="J26">
-        <v>6.8650000000000002</v>
-      </c>
-      <c r="K26">
-        <v>120</v>
-      </c>
-      <c r="L26">
-        <v>622</v>
-      </c>
-      <c r="M26" s="17">
-        <f t="shared" si="16"/>
-        <v>1445.8000000000002</v>
-      </c>
-      <c r="N26" s="17">
-        <f t="shared" si="17"/>
-        <v>168.6766666666667</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B27">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>157</v>
       </c>
       <c r="D27" t="s">
+        <v>136</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="I27" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="J27">
+        <v>6.8650000000000002</v>
+      </c>
+      <c r="K27">
+        <v>120</v>
+      </c>
+      <c r="L27">
+        <v>622</v>
+      </c>
+      <c r="M27" s="17">
+        <f t="shared" si="18"/>
+        <v>1445.8000000000002</v>
+      </c>
+      <c r="N27" s="17">
+        <f t="shared" si="19"/>
+        <v>168.6766666666667</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="40"/>
+      <c r="B28" s="40">
+        <v>0</v>
+      </c>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40" t="s">
         <v>165</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="E28" s="40"/>
+      <c r="F28" s="41" t="s">
         <v>164</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G28" s="41" t="s">
         <v>163</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="H28" s="41" t="s">
         <v>161</v>
       </c>
-      <c r="I27" s="18" t="s">
+      <c r="I28" s="42" t="s">
         <v>162</v>
       </c>
-      <c r="J27">
+      <c r="J28" s="40">
         <v>5</v>
       </c>
-      <c r="K27">
+      <c r="K28" s="40">
         <v>20</v>
       </c>
-      <c r="M27" s="17">
-        <f t="shared" ref="M27:M28" si="18">J27*K27+L27</f>
+      <c r="L28" s="40"/>
+      <c r="M28" s="44">
+        <f t="shared" ref="M28:M30" si="20">J28*K28+L28</f>
         <v>100</v>
       </c>
-      <c r="N27" s="17">
-        <f t="shared" ref="N27:N28" si="19">M27/K27*B27</f>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>173</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="I28" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="J28">
-        <v>105.373</v>
-      </c>
-      <c r="K28">
-        <v>10</v>
-      </c>
-      <c r="L28">
-        <v>1021.53</v>
-      </c>
-      <c r="M28" s="17">
-        <f t="shared" si="18"/>
-        <v>2075.2600000000002</v>
-      </c>
-      <c r="N28" s="17">
-        <f t="shared" si="19"/>
-        <v>207.52600000000001</v>
+      <c r="N28" s="44">
+        <f t="shared" ref="N28:N30" si="21">M28/K28*B28</f>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>174</v>
+        <v>249</v>
       </c>
       <c r="B29">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>177</v>
-      </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="18"/>
+        <v>165</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>252</v>
+      </c>
       <c r="J29">
-        <f>4400/750</f>
-        <v>5.8666666666666663</v>
+        <v>1.3</v>
       </c>
       <c r="K29">
-        <v>750</v>
+        <v>120</v>
       </c>
       <c r="M29" s="17">
-        <f t="shared" ref="M29" si="20">J29*K29+L29</f>
-        <v>4400</v>
+        <f t="shared" si="20"/>
+        <v>156</v>
       </c>
       <c r="N29" s="17">
-        <f t="shared" ref="N29" si="21">M29/K29*B29</f>
-        <v>422.4</v>
+        <f t="shared" si="21"/>
+        <v>22.1</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>216</v>
+        <v>173</v>
       </c>
       <c r="B30">
-        <v>42</v>
-      </c>
-      <c r="D30" t="s">
-        <v>217</v>
+        <v>1</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="18"/>
+      <c r="H30" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="I30" s="18" t="s">
+        <v>176</v>
+      </c>
       <c r="J30">
-        <f>4400/750</f>
-        <v>5.8666666666666663</v>
+        <v>105.373</v>
       </c>
       <c r="K30">
-        <v>750</v>
+        <v>10</v>
+      </c>
+      <c r="L30">
+        <v>1021.53</v>
       </c>
       <c r="M30" s="17">
-        <f t="shared" ref="M30" si="22">J30*K30+L30</f>
-        <v>4400</v>
+        <f t="shared" si="20"/>
+        <v>2075.2600000000002</v>
       </c>
       <c r="N30" s="17">
-        <f t="shared" ref="N30" si="23">M30/K30*B30</f>
-        <v>246.39999999999998</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="21"/>
+        <v>207.52600000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>215</v>
+        <v>174</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>72</v>
+      </c>
+      <c r="D31" t="s">
+        <v>177</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="18"/>
       <c r="J31">
+        <f>4400/750</f>
+        <v>5.8666666666666663</v>
+      </c>
+      <c r="K31">
+        <v>750</v>
+      </c>
+      <c r="M31" s="17">
+        <f t="shared" ref="M31" si="22">J31*K31+L31</f>
+        <v>4400</v>
+      </c>
+      <c r="N31" s="17">
+        <f t="shared" ref="N31" si="23">M31/K31*B31</f>
+        <v>422.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>216</v>
+      </c>
+      <c r="B32">
+        <v>42</v>
+      </c>
+      <c r="D32" t="s">
+        <v>217</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="18"/>
+      <c r="J32">
+        <f>4400/750</f>
+        <v>5.8666666666666663</v>
+      </c>
+      <c r="K32">
+        <v>750</v>
+      </c>
+      <c r="M32" s="17">
+        <f t="shared" ref="M32" si="24">J32*K32+L32</f>
+        <v>4400</v>
+      </c>
+      <c r="N32" s="17">
+        <f t="shared" ref="N32" si="25">M32/K32*B32</f>
+        <v>246.39999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>239</v>
+      </c>
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>240</v>
+      </c>
+      <c r="E33" s="38" t="s">
+        <v>241</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="I33" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="J33">
+        <v>1.4508000000000001</v>
+      </c>
+      <c r="K33">
+        <v>100</v>
+      </c>
+      <c r="M33" s="17">
+        <f t="shared" ref="M33" si="26">J33*K33+L33</f>
+        <v>145.08000000000001</v>
+      </c>
+      <c r="N33" s="17">
+        <f t="shared" ref="N33" si="27">M33/K33*B33</f>
+        <v>8.7048000000000005</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>215</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="18"/>
+      <c r="J34">
         <v>10</v>
       </c>
-      <c r="K31">
+      <c r="K34">
         <v>1</v>
       </c>
-      <c r="M31" s="17">
-        <f t="shared" ref="M31" si="24">J31*K31+L31</f>
+      <c r="M34" s="17">
+        <f t="shared" ref="M34" si="28">J34*K34+L34</f>
         <v>10</v>
       </c>
-      <c r="N31" s="17">
-        <f t="shared" ref="N31" si="25">M31/K31*B31</f>
+      <c r="N34" s="17">
+        <f t="shared" ref="N34" si="29">M34/K34*B34</f>
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="19" t="s">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="20">
-        <f>SUM(N3:N31)</f>
-        <v>3176.3437777777776</v>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="20">
+        <f>SUM(N3:N34)</f>
+        <v>3077.3779111111112</v>
       </c>
     </row>
   </sheetData>
@@ -3932,9 +4332,9 @@
     <hyperlink ref="G12" r:id="rId24" xr:uid="{4609AE3D-19FF-5748-A0ED-DFFA91BB6055}"/>
     <hyperlink ref="F12" r:id="rId25" xr:uid="{2096A73D-4CE8-E74A-BB65-338C934E2A69}"/>
     <hyperlink ref="H12" r:id="rId26" display="https://www.terraelectronica.ru/order/07655639" xr:uid="{68792742-3611-704B-8F1F-1BC207B55561}"/>
-    <hyperlink ref="G24" r:id="rId27" xr:uid="{286DB45E-D43F-FB43-B2BF-2425FBCA18F9}"/>
-    <hyperlink ref="F24" r:id="rId28" xr:uid="{4F4D8AE5-D858-AF4E-BA90-8140DCA9B7F5}"/>
-    <hyperlink ref="H24" r:id="rId29" display="https://www.terraelectronica.ru/order/07655639" xr:uid="{85C02143-9E94-CA45-A6BA-FAC696C48A8A}"/>
+    <hyperlink ref="G25" r:id="rId27" xr:uid="{286DB45E-D43F-FB43-B2BF-2425FBCA18F9}"/>
+    <hyperlink ref="F25" r:id="rId28" xr:uid="{4F4D8AE5-D858-AF4E-BA90-8140DCA9B7F5}"/>
+    <hyperlink ref="H25" r:id="rId29" display="https://www.terraelectronica.ru/order/07655639" xr:uid="{85C02143-9E94-CA45-A6BA-FAC696C48A8A}"/>
     <hyperlink ref="G13" r:id="rId30" xr:uid="{3E564333-1F41-3B42-958E-9100A88DC0C7}"/>
     <hyperlink ref="F13" r:id="rId31" xr:uid="{5FC52C21-9DF6-A641-9A20-4B26CC96467E}"/>
     <hyperlink ref="H13" r:id="rId32" display="https://www.terraelectronica.ru/order/07655639" xr:uid="{085EB337-BEDF-314C-8812-6C18F9A4ECA9}"/>
@@ -3950,38 +4350,45 @@
     <hyperlink ref="G17" r:id="rId42" xr:uid="{BB73D28F-1947-6B46-B0CA-F8AFD9C3045D}"/>
     <hyperlink ref="F17" r:id="rId43" xr:uid="{AB9C9562-5639-1F4F-87C3-BF35D6BAF6B9}"/>
     <hyperlink ref="H17" r:id="rId44" display="https://www.terraelectronica.ru/order/07655639" xr:uid="{816F5E02-522A-5042-9A9C-46C12545D86F}"/>
-    <hyperlink ref="G25" r:id="rId45" xr:uid="{B36444DD-A6C0-D14C-BE91-16349F83E865}"/>
-    <hyperlink ref="F25" r:id="rId46" xr:uid="{677CCA7C-5BD1-964C-BD4A-6AB6EB745994}"/>
-    <hyperlink ref="H25" r:id="rId47" display="https://www.terraelectronica.ru/order/07655639" xr:uid="{A188EEAB-9F73-7F4C-841E-376D4E95898B}"/>
-    <hyperlink ref="G23" r:id="rId48" xr:uid="{23D92319-1E56-314B-BD63-1D63071B2316}"/>
-    <hyperlink ref="F23" r:id="rId49" xr:uid="{5BCC6843-4313-B14C-AF37-14DED1C8074B}"/>
-    <hyperlink ref="H23" r:id="rId50" display="https://www.terraelectronica.ru/order/07655639" xr:uid="{507759AB-974E-8A44-89BE-DAF6332DDF7E}"/>
-    <hyperlink ref="G22" r:id="rId51" xr:uid="{1AE5ADCD-35CA-1649-B222-2FB2B36A86B1}"/>
-    <hyperlink ref="F22" r:id="rId52" display="12.88009" xr:uid="{D5A32E27-4833-084F-BAB9-72768F14FA28}"/>
-    <hyperlink ref="H22" r:id="rId53" display="https://www.terraelectronica.ru/order/07655639" xr:uid="{C93D892D-7B84-BF4B-AFC8-558357942891}"/>
+    <hyperlink ref="G26" r:id="rId45" xr:uid="{B36444DD-A6C0-D14C-BE91-16349F83E865}"/>
+    <hyperlink ref="F26" r:id="rId46" xr:uid="{677CCA7C-5BD1-964C-BD4A-6AB6EB745994}"/>
+    <hyperlink ref="H26" r:id="rId47" display="https://www.terraelectronica.ru/order/07655639" xr:uid="{A188EEAB-9F73-7F4C-841E-376D4E95898B}"/>
+    <hyperlink ref="G24" r:id="rId48" xr:uid="{23D92319-1E56-314B-BD63-1D63071B2316}"/>
+    <hyperlink ref="F24" r:id="rId49" xr:uid="{5BCC6843-4313-B14C-AF37-14DED1C8074B}"/>
+    <hyperlink ref="H24" r:id="rId50" display="https://www.terraelectronica.ru/order/07655639" xr:uid="{507759AB-974E-8A44-89BE-DAF6332DDF7E}"/>
+    <hyperlink ref="G23" r:id="rId51" xr:uid="{1AE5ADCD-35CA-1649-B222-2FB2B36A86B1}"/>
+    <hyperlink ref="F23" r:id="rId52" display="12.88009" xr:uid="{D5A32E27-4833-084F-BAB9-72768F14FA28}"/>
+    <hyperlink ref="H23" r:id="rId53" display="https://www.terraelectronica.ru/order/07655639" xr:uid="{C93D892D-7B84-BF4B-AFC8-558357942891}"/>
     <hyperlink ref="G18" r:id="rId54" xr:uid="{7E406FAF-40A8-E64D-92A0-09809FFCF5E9}"/>
     <hyperlink ref="F18" r:id="rId55" xr:uid="{46EEC713-5B53-A844-8E45-F1EE9B0A65FD}"/>
     <hyperlink ref="H18" r:id="rId56" display="https://www.terraelectronica.ru/order/07655639" xr:uid="{0E057236-AE0C-CB49-96FD-145DFF3852E4}"/>
     <hyperlink ref="G19" r:id="rId57" xr:uid="{4909AF0A-C056-3A4D-AF36-EC4BA81B1DE9}"/>
     <hyperlink ref="F19" r:id="rId58" xr:uid="{1C145889-FA2F-124D-80FB-B4700BDF4912}"/>
     <hyperlink ref="H19" r:id="rId59" xr:uid="{AED11A1F-1D82-A241-B5D7-9551791987BE}"/>
-    <hyperlink ref="G21" r:id="rId60" xr:uid="{4D35C340-51A2-4848-93D7-95D6FE3C9775}"/>
-    <hyperlink ref="F21" r:id="rId61" xr:uid="{FBB1AA98-E1E8-7343-895B-BC794ACB8BB9}"/>
-    <hyperlink ref="H21" r:id="rId62" xr:uid="{23C9494A-413B-5A42-BF06-B49B5684AF06}"/>
-    <hyperlink ref="H27" r:id="rId63" xr:uid="{79D106DF-5F99-E748-99DD-AC8FCA4E11D7}"/>
-    <hyperlink ref="G27" r:id="rId64" xr:uid="{4B44E84E-C5AE-E240-A016-118DA8089AA7}"/>
-    <hyperlink ref="F27" r:id="rId65" xr:uid="{42C4ADBD-C016-7440-B6D4-5324C15A646D}"/>
+    <hyperlink ref="G22" r:id="rId60" xr:uid="{4D35C340-51A2-4848-93D7-95D6FE3C9775}"/>
+    <hyperlink ref="F22" r:id="rId61" xr:uid="{FBB1AA98-E1E8-7343-895B-BC794ACB8BB9}"/>
+    <hyperlink ref="H22" r:id="rId62" xr:uid="{23C9494A-413B-5A42-BF06-B49B5684AF06}"/>
+    <hyperlink ref="H28" r:id="rId63" xr:uid="{79D106DF-5F99-E748-99DD-AC8FCA4E11D7}"/>
+    <hyperlink ref="G28" r:id="rId64" xr:uid="{4B44E84E-C5AE-E240-A016-118DA8089AA7}"/>
+    <hyperlink ref="F28" r:id="rId65" xr:uid="{42C4ADBD-C016-7440-B6D4-5324C15A646D}"/>
     <hyperlink ref="G20" r:id="rId66" xr:uid="{93DA5CD1-ABEF-674D-9212-FAE2AE2BF654}"/>
     <hyperlink ref="F20" r:id="rId67" xr:uid="{30AA4905-E0FF-6549-9069-F462D5C4A1BD}"/>
     <hyperlink ref="H20" r:id="rId68" xr:uid="{A323439E-F4BA-D045-9CFB-9F6F674F97D5}"/>
-    <hyperlink ref="G26" r:id="rId69" xr:uid="{855F3123-A9C8-F140-B301-258524A8A90A}"/>
-    <hyperlink ref="H26" r:id="rId70" xr:uid="{2F8DF8A3-A5E4-484B-AA6C-B2FFF2BD2142}"/>
-    <hyperlink ref="F26" r:id="rId71" xr:uid="{B3CD6BF5-783D-844F-8A0B-75F3737D466E}"/>
-    <hyperlink ref="H28" r:id="rId72" xr:uid="{30BDDFCA-881E-8543-B321-830CAC91976D}"/>
+    <hyperlink ref="G27" r:id="rId69" xr:uid="{855F3123-A9C8-F140-B301-258524A8A90A}"/>
+    <hyperlink ref="H27" r:id="rId70" xr:uid="{2F8DF8A3-A5E4-484B-AA6C-B2FFF2BD2142}"/>
+    <hyperlink ref="F27" r:id="rId71" xr:uid="{B3CD6BF5-783D-844F-8A0B-75F3737D466E}"/>
+    <hyperlink ref="H30" r:id="rId72" xr:uid="{30BDDFCA-881E-8543-B321-830CAC91976D}"/>
     <hyperlink ref="G3" r:id="rId73" xr:uid="{72CB063E-DC65-3C4D-B1ED-4612847366F7}"/>
     <hyperlink ref="F3" r:id="rId74" xr:uid="{013BCB57-B05C-AF48-BAF4-448E5DC6E0FF}"/>
     <hyperlink ref="H11" r:id="rId75" xr:uid="{655965E6-46F6-D746-BC91-1FE006B4ADB4}"/>
     <hyperlink ref="H3" r:id="rId76" xr:uid="{48EE2201-84CE-8B4F-91B5-D13A630F7858}"/>
+    <hyperlink ref="F21" r:id="rId77" xr:uid="{48328A4D-ADB7-8B40-A686-B975DBFA7271}"/>
+    <hyperlink ref="H21" r:id="rId78" xr:uid="{B07D6D76-69D2-2A4D-998D-F12B31F8C0FD}"/>
+    <hyperlink ref="F29" r:id="rId79" xr:uid="{7B89F9D1-2FF8-3848-94CC-7D51DCC572B2}"/>
+    <hyperlink ref="G29" r:id="rId80" xr:uid="{71ABF7A8-4763-C349-A03A-25AE08F8A86E}"/>
+    <hyperlink ref="H29" r:id="rId81" xr:uid="{1B3EB5E5-028F-904F-8239-15D309692A51}"/>
+    <hyperlink ref="F33" r:id="rId82" xr:uid="{DDEB64EF-A01D-EE48-897E-97A74563D9FC}"/>
+    <hyperlink ref="H33" r:id="rId83" xr:uid="{06B468F3-4351-0F4D-848F-3DE0082A9A95}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>